<commit_message>
Rebecca updated the backlog.  -Angie
</commit_message>
<xml_diff>
--- a/CPSC350SprintBacklog.xlsx
+++ b/CPSC350SprintBacklog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680"/>
+    <workbookView xWindow="360" yWindow="180" windowWidth="14355" windowHeight="4620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Backlog</t>
   </si>
@@ -30,34 +30,61 @@
     <t>Posted</t>
   </si>
   <si>
-    <t>setup data base</t>
-  </si>
-  <si>
-    <t>setup git repos.</t>
-  </si>
-  <si>
-    <t>setup website template</t>
-  </si>
-  <si>
     <t>Sprint Backlog</t>
   </si>
   <si>
-    <t>setup data base(Angie)</t>
-  </si>
-  <si>
-    <t>setup website template( James&amp; Rebecca)</t>
-  </si>
-  <si>
-    <t>setup git repos. (BEN)</t>
-  </si>
-  <si>
-    <t>repos. Made adding members</t>
-  </si>
-  <si>
-    <t>database setup( angie, me)</t>
-  </si>
-  <si>
-    <t>website design/product choices (Ben and James)</t>
+    <t>rewrite repo to clean it up (Ben)</t>
+  </si>
+  <si>
+    <t>Straigten up database (Rebecca)</t>
+  </si>
+  <si>
+    <t>Website update(Ben and James)</t>
+  </si>
+  <si>
+    <t>Update orderform (James)</t>
+  </si>
+  <si>
+    <t>cleanup home page design (Ben)</t>
+  </si>
+  <si>
+    <t>instruction written(Angie)</t>
+  </si>
+  <si>
+    <t>order form redesign (James)</t>
+  </si>
+  <si>
+    <t>clean up repo (BEN)</t>
+  </si>
+  <si>
+    <t>Database tables (Rebeca)</t>
+  </si>
+  <si>
+    <t>Add verbage to about page -angie</t>
+  </si>
+  <si>
+    <t>queries into database -rebecca and james</t>
+  </si>
+  <si>
+    <t>scout w/ most military donations- Angie</t>
+  </si>
+  <si>
+    <t>rename milary donation pg-Ben</t>
+  </si>
+  <si>
+    <t>Scout w/ most orders-ben</t>
+  </si>
+  <si>
+    <t>participating packs- Rebecca</t>
+  </si>
+  <si>
+    <t>add column for troops into scout table</t>
+  </si>
+  <si>
+    <t>add column for troops into scout table-Rebecca</t>
+  </si>
+  <si>
+    <t>increase price amount- Angie</t>
   </si>
 </sst>
 </file>
@@ -102,7 +129,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -405,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F4"/>
+  <dimension ref="B1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C14" sqref="C13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +448,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -433,15 +460,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>4</v>
+    <row r="2" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="60" x14ac:dyDescent="0.25">
@@ -449,21 +476,73 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated backlog - Angie
</commit_message>
<xml_diff>
--- a/CPSC350SprintBacklog.xlsx
+++ b/CPSC350SprintBacklog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="180" windowWidth="14355" windowHeight="4620"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>Backlog</t>
   </si>
@@ -33,65 +33,35 @@
     <t>Sprint Backlog</t>
   </si>
   <si>
-    <t>rewrite repo to clean it up (Ben)</t>
-  </si>
-  <si>
-    <t>Straigten up database (Rebecca)</t>
-  </si>
-  <si>
-    <t>Website update(Ben and James)</t>
-  </si>
-  <si>
-    <t>Update orderform (James)</t>
-  </si>
-  <si>
-    <t>cleanup home page design (Ben)</t>
-  </si>
-  <si>
-    <t>instruction written(Angie)</t>
-  </si>
-  <si>
-    <t>order form redesign (James)</t>
-  </si>
-  <si>
-    <t>clean up repo (BEN)</t>
-  </si>
-  <si>
-    <t>Database tables (Rebeca)</t>
-  </si>
-  <si>
-    <t>Add verbage to about page -angie</t>
-  </si>
-  <si>
-    <t>queries into database -rebecca and james</t>
-  </si>
-  <si>
-    <t>scout w/ most military donations- Angie</t>
-  </si>
-  <si>
-    <t>rename milary donation pg-Ben</t>
-  </si>
-  <si>
-    <t>Scout w/ most orders-ben</t>
-  </si>
-  <si>
-    <t>participating packs- Rebecca</t>
-  </si>
-  <si>
-    <t>add column for troops into scout table</t>
-  </si>
-  <si>
-    <t>add column for troops into scout table-Rebecca</t>
-  </si>
-  <si>
-    <t>increase price amount- Angie</t>
+    <t>correct sub-title on home pg (BEN)</t>
+  </si>
+  <si>
+    <t>create contact pg (Angie)</t>
+  </si>
+  <si>
+    <t>Confirm format (all)</t>
+  </si>
+  <si>
+    <t>Update price field (Angie)</t>
+  </si>
+  <si>
+    <t>Query scout with most sales (Jim)</t>
+  </si>
+  <si>
+    <t>Testing(Angie)</t>
+  </si>
+  <si>
+    <t>Rewrite queries(all)</t>
+  </si>
+  <si>
+    <t>3NF tables w/ JOINS (Rebecca)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,7 +190,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -255,7 +224,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -431,19 +399,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C13:C14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -460,90 +428,94 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" ht="45">
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="2:6" ht="30">
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="2:6" ht="30">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="2:6" ht="30">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="2:6" ht="45">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="2:6" ht="26.25" customHeight="1">
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="30">
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="C11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="F13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -551,24 +523,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>